<commit_message>
Updated Black box test cases
</commit_message>
<xml_diff>
--- a/src/BlackBoxTestCases.xlsx
+++ b/src/BlackBoxTestCases.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CollegeWork\CollegeY4\VerificationRepeat\RepeatVerificationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFBEFB8-771E-4CE5-A1B0-BAD9B83F820C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008D92C-5BFC-4810-A90C-8F5E6AAAD27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BlackBox" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -193,12 +193,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -233,11 +239,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,8 +563,8 @@
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -575,295 +581,293 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="D21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D24" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D25" s="4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>